<commit_message>
UP-Sell and Customer Churn test cases added
</commit_message>
<xml_diff>
--- a/testData/qa/up_sell.xlsx
+++ b/testData/qa/up_sell.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naga.kumar\OneDrive - ElectrifAI\newuiautomation\testData\qa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naga.kumar\customerAi\testData\qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99099895-7333-484F-8EA0-DD471DEA706E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F2089C-0CD1-40B6-85E1-0C2793CCBC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EE76EA1F-E72F-46B2-BEA2-9E761BC260D6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{EE76EA1F-E72F-46B2-BEA2-9E761BC260D6}"/>
   </bookViews>
   <sheets>
     <sheet name="up_sell_Filter" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>DataRowNum</t>
   </si>
@@ -114,19 +114,37 @@
     <t>Profiles for Top 75% to 90%</t>
   </si>
   <si>
+    <t>Deposit Account</t>
+  </si>
+  <si>
+    <t>Within 90 days</t>
+  </si>
+  <si>
+    <t>Overall</t>
+  </si>
+  <si>
+    <t>Driver 1,Driver 2,Driver 3,Driver 4,Driver 5</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Selected Drivers</t>
+  </si>
+  <si>
     <t>Product Up-Sell Drivers for Top 90% to 100%</t>
   </si>
   <si>
     <t>Product Up-Sell Drivers for Top 75% to 100%</t>
   </si>
   <si>
+    <t>Product Up-Sell Drivers for Top 50% to 75%</t>
+  </si>
+  <si>
+    <t>Product Up-Sell Drivers for Top 75% to 90%</t>
+  </si>
+  <si>
     <t>Product Up-Sell Drivers for Top 50% to 100%</t>
-  </si>
-  <si>
-    <t>Product Up-Sell Drivers for Top 50% to 75%</t>
-  </si>
-  <si>
-    <t>Product Up-Sell Drivers for Top 75% to 90%</t>
   </si>
 </sst>
 </file>
@@ -521,25 +539,25 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="41.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.453125" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -553,11 +571,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
@@ -566,9 +586,17 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="C3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -578,22 +606,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D519C6-B5E4-4FAF-A519-D5C875BF9495}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.54296875" customWidth="1"/>
+    <col min="5" max="5" width="35.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -604,13 +633,16 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -621,13 +653,16 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -638,30 +673,36 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -672,13 +713,16 @@
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -692,24 +736,30 @@
         <v>29</v>
       </c>
       <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>